<commit_message>
mixed channel images create patches now return 3 channel
</commit_message>
<xml_diff>
--- a/evaluation/training-evaluation.xlsx
+++ b/evaluation/training-evaluation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - University of Cyprus\ucl\thesis\workspace\cell-tracking-ucl-thesis\evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DC5A2E-0786-49B8-9E40-7C583E11399D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8F5600-FAA6-4EF1-810D-025292F001D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{DD5E1588-BB96-47E2-8F58-F1B1A8926599}"/>
   </bookViews>
@@ -87,7 +87,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +102,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="4"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,9 +130,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25252485-713D-4CC8-BE64-95040359BD5A}">
-  <dimension ref="A1:K79"/>
+  <dimension ref="A1:K110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="H75" sqref="H75"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="P77" sqref="P77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -705,16 +714,16 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0.89200000000000002</v>
+        <v>0.86</v>
       </c>
       <c r="I15">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="J15">
         <v>0.83099999999999996</v>
       </c>
-      <c r="J15">
-        <v>0.84899999999999998</v>
-      </c>
       <c r="K15">
-        <v>0.91100000000000003</v>
+        <v>0.88100000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -731,16 +740,16 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0.874</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="I16">
-        <v>0.85299999999999998</v>
+        <v>0.83699999999999997</v>
       </c>
       <c r="J16">
-        <v>0.88300000000000001</v>
+        <v>0.85</v>
       </c>
       <c r="K16">
-        <v>0.85599999999999998</v>
+        <v>0.91800000000000004</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -757,16 +766,16 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0.85699999999999998</v>
+        <v>0.89200000000000002</v>
       </c>
       <c r="I17">
-        <v>0.83399999999999996</v>
+        <v>0.83099999999999996</v>
       </c>
       <c r="J17">
-        <v>0.82899999999999996</v>
+        <v>0.84899999999999998</v>
       </c>
       <c r="K17">
-        <v>0.875</v>
+        <v>0.91100000000000003</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -783,16 +792,16 @@
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0.86499999999999999</v>
+        <v>0.874</v>
       </c>
       <c r="I18">
-        <v>0.83799999999999997</v>
+        <v>0.85299999999999998</v>
       </c>
       <c r="J18">
-        <v>0.83299999999999996</v>
+        <v>0.88300000000000001</v>
       </c>
       <c r="K18">
-        <v>0.88700000000000001</v>
+        <v>0.85599999999999998</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -809,86 +818,86 @@
         <v>0</v>
       </c>
       <c r="H19">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="I19">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="J19">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="K19">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="b">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>31</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="I20">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="J20">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="K20">
+        <v>0.88700000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="b">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>31</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21">
         <v>0.89200000000000002</v>
       </c>
-      <c r="I19">
+      <c r="I21">
         <v>0.83099999999999996</v>
       </c>
-      <c r="J19">
+      <c r="J21">
         <v>0.84899999999999998</v>
       </c>
-      <c r="K19">
+      <c r="K21">
         <v>0.91100000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H20">
-        <f>AVERAGE(H15:H19)</f>
-        <v>0.87600000000000011</v>
-      </c>
-      <c r="I20">
-        <f t="shared" ref="I20:K20" si="2">AVERAGE(I15:I19)</f>
-        <v>0.83739999999999992</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="2"/>
-        <v>0.84860000000000002</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="2"/>
-        <v>0.8879999999999999</v>
-      </c>
-    </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="b">
-        <v>1</v>
-      </c>
-      <c r="B22">
-        <v>31</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22" t="b">
-        <v>0</v>
-      </c>
       <c r="H22">
-        <v>0.89</v>
+        <f>AVERAGE(H15:H21)</f>
+        <v>0.87642857142857156</v>
       </c>
       <c r="I22">
-        <v>0.84399999999999997</v>
+        <f>AVERAGE(I15:I21)</f>
+        <v>0.83757142857142852</v>
       </c>
       <c r="J22">
-        <v>0.92700000000000005</v>
+        <f>AVERAGE(J15:J21)</f>
+        <v>0.84628571428571431</v>
       </c>
       <c r="K22">
-        <v>0.83499999999999996</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="b">
-        <v>1</v>
-      </c>
-      <c r="B23">
-        <v>31</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0.88300000000000001</v>
-      </c>
-      <c r="I23">
-        <v>0.84</v>
-      </c>
-      <c r="J23">
-        <v>0.89800000000000002</v>
-      </c>
-      <c r="K23">
-        <v>0.85199999999999998</v>
+        <f>AVERAGE(K15:K21)</f>
+        <v>0.89128571428571413</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -905,16 +914,16 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <v>0.86499999999999999</v>
+        <v>0.89</v>
       </c>
       <c r="I24">
-        <v>0.83399999999999996</v>
+        <v>0.84399999999999997</v>
       </c>
       <c r="J24">
-        <v>0.86799999999999999</v>
+        <v>0.92700000000000005</v>
       </c>
       <c r="K24">
-        <v>0.85</v>
+        <v>0.83499999999999996</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -931,16 +940,16 @@
         <v>0</v>
       </c>
       <c r="H25">
-        <v>0.878</v>
+        <v>0.88300000000000001</v>
       </c>
       <c r="I25">
-        <v>0.84299999999999997</v>
+        <v>0.84</v>
       </c>
       <c r="J25">
-        <v>0.85</v>
+        <v>0.89800000000000002</v>
       </c>
       <c r="K25">
-        <v>0.89200000000000002</v>
+        <v>0.85199999999999998</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -957,114 +966,108 @@
         <v>0</v>
       </c>
       <c r="H26">
-        <v>0.85699999999999998</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="I26">
         <v>0.83399999999999996</v>
       </c>
       <c r="J26">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="K26">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="b">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>31</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0.878</v>
+      </c>
+      <c r="I27">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="J27">
+        <v>0.85</v>
+      </c>
+      <c r="K27">
+        <v>0.89200000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="b">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>31</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="I28">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="J28">
         <v>0.82899999999999996</v>
       </c>
-      <c r="K26">
+      <c r="K28">
         <v>0.875</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H27">
-        <f>AVERAGE(H22:H26)</f>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="H29">
+        <f>AVERAGE(H24:H28)</f>
         <v>0.87460000000000004</v>
       </c>
-      <c r="I27">
-        <f t="shared" ref="I27:K27" si="3">AVERAGE(I22:I26)</f>
+      <c r="I29">
+        <f t="shared" ref="I29:K29" si="2">AVERAGE(I24:I28)</f>
         <v>0.83899999999999986</v>
       </c>
-      <c r="J27">
-        <f t="shared" si="3"/>
+      <c r="J29">
+        <f t="shared" si="2"/>
         <v>0.87439999999999996</v>
       </c>
-      <c r="K27">
-        <f t="shared" si="3"/>
+      <c r="K29">
+        <f t="shared" si="2"/>
         <v>0.86080000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="1" t="s">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
         <v>2</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D36" t="s">
         <v>3</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E36" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="b">
-        <v>1</v>
-      </c>
-      <c r="B35">
-        <v>15</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35" t="b">
-        <v>0</v>
-      </c>
-      <c r="E35" t="b">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0.81599999999999995</v>
-      </c>
-      <c r="I35">
-        <v>0.81599999999999995</v>
-      </c>
-      <c r="J35">
-        <v>0.78800000000000003</v>
-      </c>
-      <c r="K35">
-        <v>0.84299999999999997</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="b">
-        <v>1</v>
-      </c>
-      <c r="B36">
-        <v>15</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E36" t="b">
-        <v>0</v>
-      </c>
-      <c r="H36">
-        <v>0.80900000000000005</v>
-      </c>
-      <c r="I36">
-        <v>0.80300000000000005</v>
-      </c>
-      <c r="J36">
-        <v>0.749</v>
-      </c>
-      <c r="K36">
-        <v>0.86699999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1084,92 +1087,92 @@
         <v>0</v>
       </c>
       <c r="H37">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="I37">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="J37">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="K37">
+        <v>0.84299999999999997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="b">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>15</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" t="b">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="I38">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="J38">
+        <v>0.749</v>
+      </c>
+      <c r="K38">
+        <v>0.86699999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="b">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>15</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" t="b">
+        <v>0</v>
+      </c>
+      <c r="H39">
         <v>0.83499999999999996</v>
       </c>
-      <c r="I37">
+      <c r="I39">
         <v>0.81299999999999994</v>
       </c>
-      <c r="J37">
+      <c r="J39">
         <v>0.86</v>
       </c>
-      <c r="K37">
+      <c r="K39">
         <v>0.80100000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H38">
-        <f>AVERAGE(H35:H37)</f>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="H40">
+        <f>AVERAGE(H37:H39)</f>
         <v>0.82</v>
       </c>
-      <c r="I38">
-        <f t="shared" ref="I38:K38" si="4">AVERAGE(I35:I37)</f>
+      <c r="I40">
+        <f t="shared" ref="I40:K40" si="3">AVERAGE(I37:I39)</f>
         <v>0.81066666666666665</v>
       </c>
-      <c r="J38">
-        <f t="shared" si="4"/>
+      <c r="J40">
+        <f t="shared" si="3"/>
         <v>0.79899999999999993</v>
       </c>
-      <c r="K38">
-        <f t="shared" si="4"/>
+      <c r="K40">
+        <f t="shared" si="3"/>
         <v>0.83700000000000008</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" t="b">
-        <v>1</v>
-      </c>
-      <c r="B40">
-        <v>17</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" t="b">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>0.84099999999999997</v>
-      </c>
-      <c r="I40">
-        <v>0.82299999999999995</v>
-      </c>
-      <c r="J40">
-        <v>0.83599999999999997</v>
-      </c>
-      <c r="K40">
-        <v>0.83799999999999997</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" t="b">
-        <v>1</v>
-      </c>
-      <c r="B41">
-        <v>17</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-      <c r="D41" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" t="b">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0.83</v>
-      </c>
-      <c r="I41">
-        <v>0.81299999999999994</v>
-      </c>
-      <c r="J41">
-        <v>0.85799999999999998</v>
-      </c>
-      <c r="K41">
-        <v>0.79500000000000004</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1192,13 +1195,13 @@
         <v>0.84099999999999997</v>
       </c>
       <c r="I42">
-        <v>0.81100000000000005</v>
+        <v>0.82299999999999995</v>
       </c>
       <c r="J42">
-        <v>0.87</v>
+        <v>0.83599999999999997</v>
       </c>
       <c r="K42">
-        <v>0.80100000000000005</v>
+        <v>0.83799999999999997</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1218,16 +1221,16 @@
         <v>0</v>
       </c>
       <c r="H43">
-        <v>0.83799999999999997</v>
+        <v>0.83</v>
       </c>
       <c r="I43">
         <v>0.81299999999999994</v>
       </c>
       <c r="J43">
-        <v>0.78900000000000003</v>
+        <v>0.85799999999999998</v>
       </c>
       <c r="K43">
-        <v>0.877</v>
+        <v>0.79500000000000004</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1247,92 +1250,92 @@
         <v>0</v>
       </c>
       <c r="H44">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="I44">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="J44">
+        <v>0.87</v>
+      </c>
+      <c r="K44">
+        <v>0.80100000000000005</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="b">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>17</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45" t="b">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="I45">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="J45">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="K45">
+        <v>0.877</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="b">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>17</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H46">
         <v>0.82</v>
       </c>
-      <c r="I44">
+      <c r="I46">
         <v>0.81</v>
       </c>
-      <c r="J44">
+      <c r="J46">
         <v>0.871</v>
       </c>
-      <c r="K44">
+      <c r="K46">
         <v>0.76500000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H45">
-        <f>AVERAGE(H40:H44)</f>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="H47">
+        <f>AVERAGE(H42:H46)</f>
         <v>0.83399999999999996</v>
       </c>
-      <c r="I45">
-        <f t="shared" ref="I45:K45" si="5">AVERAGE(I40:I44)</f>
+      <c r="I47">
+        <f t="shared" ref="I47:K47" si="4">AVERAGE(I42:I46)</f>
         <v>0.81400000000000006</v>
       </c>
-      <c r="J45">
-        <f t="shared" si="5"/>
+      <c r="J47">
+        <f t="shared" si="4"/>
         <v>0.8448</v>
       </c>
-      <c r="K45">
-        <f t="shared" si="5"/>
+      <c r="K47">
+        <f t="shared" si="4"/>
         <v>0.81519999999999992</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" t="b">
-        <v>1</v>
-      </c>
-      <c r="B47">
-        <v>19</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-      <c r="D47" t="b">
-        <v>0</v>
-      </c>
-      <c r="E47" t="b">
-        <v>0</v>
-      </c>
-      <c r="H47">
-        <v>0.82699999999999996</v>
-      </c>
-      <c r="I47">
-        <v>0.81699999999999995</v>
-      </c>
-      <c r="J47">
-        <v>0.83099999999999996</v>
-      </c>
-      <c r="K47">
-        <v>0.81899999999999995</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" t="b">
-        <v>1</v>
-      </c>
-      <c r="B48">
-        <v>19</v>
-      </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-      <c r="D48" t="b">
-        <v>0</v>
-      </c>
-      <c r="E48" t="b">
-        <v>0</v>
-      </c>
-      <c r="H48">
-        <v>0.82399999999999995</v>
-      </c>
-      <c r="I48">
-        <v>0.82299999999999995</v>
-      </c>
-      <c r="J48">
-        <v>0.82699999999999996</v>
-      </c>
-      <c r="K48">
-        <v>0.82099999999999995</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1352,16 +1355,16 @@
         <v>0</v>
       </c>
       <c r="H49">
-        <v>0.82599999999999996</v>
+        <v>0.82699999999999996</v>
       </c>
       <c r="I49">
-        <v>0.81399999999999995</v>
+        <v>0.81699999999999995</v>
       </c>
       <c r="J49">
-        <v>0.749</v>
+        <v>0.83099999999999996</v>
       </c>
       <c r="K49">
-        <v>0.89900000000000002</v>
+        <v>0.81899999999999995</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1381,92 +1384,92 @@
         <v>0</v>
       </c>
       <c r="H50">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="I50">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="J50">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="K50">
+        <v>0.82099999999999995</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="b">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>19</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="I51">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="J51">
+        <v>0.749</v>
+      </c>
+      <c r="K51">
+        <v>0.89900000000000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="b">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>19</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" t="b">
+        <v>0</v>
+      </c>
+      <c r="H52">
         <v>0.83199999999999996</v>
       </c>
-      <c r="I50">
+      <c r="I52">
         <v>0.82199999999999995</v>
       </c>
-      <c r="J50">
+      <c r="J52">
         <v>0.85899999999999999</v>
       </c>
-      <c r="K50">
+      <c r="K52">
         <v>0.80100000000000005</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H51">
-        <f>AVERAGE(H47:H50)</f>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="H53">
+        <f>AVERAGE(H49:H52)</f>
         <v>0.82724999999999993</v>
       </c>
-      <c r="I51">
-        <f t="shared" ref="I51:K51" si="6">AVERAGE(I47:I50)</f>
+      <c r="I53">
+        <f t="shared" ref="I53:K53" si="5">AVERAGE(I49:I52)</f>
         <v>0.81899999999999995</v>
       </c>
-      <c r="J51">
-        <f t="shared" si="6"/>
+      <c r="J53">
+        <f t="shared" si="5"/>
         <v>0.8165</v>
       </c>
-      <c r="K51">
-        <f t="shared" si="6"/>
+      <c r="K53">
+        <f t="shared" si="5"/>
         <v>0.83499999999999996</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" t="b">
-        <v>1</v>
-      </c>
-      <c r="B53">
-        <v>21</v>
-      </c>
-      <c r="C53">
-        <v>0</v>
-      </c>
-      <c r="D53" t="b">
-        <v>0</v>
-      </c>
-      <c r="E53" t="b">
-        <v>0</v>
-      </c>
-      <c r="H53">
-        <v>0.84499999999999997</v>
-      </c>
-      <c r="I53">
-        <v>0.82199999999999995</v>
-      </c>
-      <c r="J53">
-        <v>0.89500000000000002</v>
-      </c>
-      <c r="K53">
-        <v>0.78700000000000003</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" t="b">
-        <v>1</v>
-      </c>
-      <c r="B54">
-        <v>21</v>
-      </c>
-      <c r="C54">
-        <v>0</v>
-      </c>
-      <c r="D54" t="b">
-        <v>0</v>
-      </c>
-      <c r="E54" t="b">
-        <v>0</v>
-      </c>
-      <c r="H54">
-        <v>0.82399999999999995</v>
-      </c>
-      <c r="I54">
-        <v>0.80700000000000005</v>
-      </c>
-      <c r="J54">
-        <v>0.76100000000000001</v>
-      </c>
-      <c r="K54">
-        <v>0.88100000000000001</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1486,16 +1489,16 @@
         <v>0</v>
       </c>
       <c r="H55">
-        <v>0.82499999999999996</v>
+        <v>0.84499999999999997</v>
       </c>
       <c r="I55">
-        <v>0.81399999999999995</v>
+        <v>0.82199999999999995</v>
       </c>
       <c r="J55">
-        <v>0.77100000000000002</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="K55">
-        <v>0.875</v>
+        <v>0.78700000000000003</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1515,68 +1518,92 @@
         <v>0</v>
       </c>
       <c r="H56">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="I56">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="J56">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="K56">
+        <v>0.88100000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="b">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>21</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" t="b">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="I57">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="J57">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="K57">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="b">
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <v>21</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" t="b">
+        <v>0</v>
+      </c>
+      <c r="H58">
         <v>0.84</v>
       </c>
-      <c r="I56">
+      <c r="I58">
         <v>0.82</v>
       </c>
-      <c r="J56">
+      <c r="J58">
         <v>0.85099999999999998</v>
       </c>
-      <c r="K56">
+      <c r="K58">
         <v>0.82099999999999995</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H57">
-        <f t="shared" ref="H57:I57" si="7">AVERAGE(H53:H56)</f>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="H59">
+        <f t="shared" ref="H59:I59" si="6">AVERAGE(H55:H58)</f>
         <v>0.83349999999999991</v>
       </c>
-      <c r="I57">
-        <f t="shared" si="7"/>
+      <c r="I59">
+        <f t="shared" si="6"/>
         <v>0.81574999999999998</v>
       </c>
-      <c r="J57">
-        <f>AVERAGE(J53:J56)</f>
+      <c r="J59">
+        <f>AVERAGE(J55:J58)</f>
         <v>0.81950000000000001</v>
       </c>
-      <c r="K57">
-        <f>AVERAGE(K53:K56)</f>
+      <c r="K59">
+        <f>AVERAGE(K55:K58)</f>
         <v>0.84099999999999997</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" t="s">
-        <v>0</v>
-      </c>
-      <c r="B60" t="s">
-        <v>1</v>
-      </c>
-      <c r="C60" t="s">
-        <v>2</v>
-      </c>
-      <c r="D60" t="s">
-        <v>3</v>
-      </c>
-      <c r="E60" t="s">
-        <v>14</v>
-      </c>
-      <c r="H60" t="s">
-        <v>4</v>
-      </c>
-      <c r="I60" t="s">
-        <v>5</v>
-      </c>
-      <c r="J60" t="s">
-        <v>6</v>
-      </c>
-      <c r="K60" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1584,7 +1611,7 @@
         <v>1</v>
       </c>
       <c r="B61">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1593,19 +1620,19 @@
         <v>0</v>
       </c>
       <c r="E61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H61">
-        <v>0.90300000000000002</v>
+        <v>0.85599999999999998</v>
       </c>
       <c r="I61">
-        <v>0.84699999999999998</v>
+        <v>0.83099999999999996</v>
       </c>
       <c r="J61">
-        <v>0.91800000000000004</v>
+        <v>0.83899999999999997</v>
       </c>
       <c r="K61">
-        <v>0.86599999999999999</v>
+        <v>0.86199999999999999</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1613,7 +1640,7 @@
         <v>1</v>
       </c>
       <c r="B62">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1622,19 +1649,19 @@
         <v>0</v>
       </c>
       <c r="E62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62">
-        <v>0.92500000000000004</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="I62">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="J62">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="K62">
         <v>0.85</v>
-      </c>
-      <c r="J62">
-        <v>0.92400000000000004</v>
-      </c>
-      <c r="K62">
-        <v>0.89500000000000002</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1642,7 +1669,7 @@
         <v>1</v>
       </c>
       <c r="B63">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1651,19 +1678,19 @@
         <v>0</v>
       </c>
       <c r="E63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H63">
-        <v>0.88600000000000001</v>
+        <v>0.85199999999999998</v>
       </c>
       <c r="I63">
-        <v>0.85199999999999998</v>
+        <v>0.82399999999999995</v>
       </c>
       <c r="J63">
-        <v>0.89200000000000002</v>
+        <v>0.88200000000000001</v>
       </c>
       <c r="K63">
-        <v>0.86699999999999999</v>
+        <v>0.81200000000000006</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1671,7 +1698,7 @@
         <v>1</v>
       </c>
       <c r="B64">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1680,77 +1707,37 @@
         <v>0</v>
       </c>
       <c r="E64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64">
-        <v>0.88400000000000001</v>
+        <v>0.83199999999999996</v>
       </c>
       <c r="I64">
-        <v>0.85</v>
+        <v>0.83199999999999996</v>
       </c>
       <c r="J64">
-        <v>0.9</v>
+        <v>0.78200000000000003</v>
       </c>
       <c r="K64">
-        <v>0.85399999999999998</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" t="b">
-        <v>1</v>
-      </c>
-      <c r="B65">
-        <v>31</v>
-      </c>
-      <c r="C65">
-        <v>0</v>
-      </c>
-      <c r="D65" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" t="b">
-        <v>1</v>
-      </c>
       <c r="H65">
-        <v>0.9</v>
+        <f>AVERAGE(H61:H64)</f>
+        <v>0.84974999999999989</v>
       </c>
       <c r="I65">
-        <v>0.86</v>
+        <f t="shared" ref="I65" si="7">AVERAGE(I61:I64)</f>
+        <v>0.83024999999999993</v>
       </c>
       <c r="J65">
-        <v>0.91100000000000003</v>
+        <f>AVERAGE(J61:J64)</f>
+        <v>0.84025000000000005</v>
       </c>
       <c r="K65">
-        <v>0.873</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" t="b">
-        <v>1</v>
-      </c>
-      <c r="B66">
-        <v>31</v>
-      </c>
-      <c r="C66">
-        <v>0</v>
-      </c>
-      <c r="D66" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" t="b">
-        <v>1</v>
-      </c>
-      <c r="H66">
-        <v>0.88300000000000001</v>
-      </c>
-      <c r="I66">
-        <v>0.84399999999999997</v>
-      </c>
-      <c r="J66">
-        <v>0.877</v>
-      </c>
-      <c r="K66">
-        <v>0.873</v>
+        <f>AVERAGE(K61:K64)</f>
+        <v>0.85099999999999998</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1767,153 +1754,870 @@
         <v>0</v>
       </c>
       <c r="E67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67">
-        <v>0.86099999999999999</v>
+        <v>0.89</v>
       </c>
       <c r="I67">
         <v>0.84399999999999997</v>
       </c>
       <c r="J67">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="K67">
+        <v>0.83499999999999996</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" t="b">
+        <v>1</v>
+      </c>
+      <c r="B68">
+        <v>31</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" t="b">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="I68">
+        <v>0.84</v>
+      </c>
+      <c r="J68">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="K68">
+        <v>0.85199999999999998</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" t="b">
+        <v>1</v>
+      </c>
+      <c r="B69">
+        <v>31</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" t="b">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="I69">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="J69">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="K69">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" t="b">
+        <v>1</v>
+      </c>
+      <c r="B70">
+        <v>31</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0.878</v>
+      </c>
+      <c r="I70">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="J70">
+        <v>0.85</v>
+      </c>
+      <c r="K70">
+        <v>0.89200000000000002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" t="b">
+        <v>1</v>
+      </c>
+      <c r="B71">
+        <v>31</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" t="b">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="I71">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="J71">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="K71">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="H72">
+        <f>AVERAGE(H67:H71)</f>
+        <v>0.87460000000000004</v>
+      </c>
+      <c r="I72">
+        <f t="shared" ref="I72:K72" si="8">AVERAGE(I67:I71)</f>
+        <v>0.83899999999999986</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="8"/>
+        <v>0.87439999999999996</v>
+      </c>
+      <c r="K72">
+        <f t="shared" si="8"/>
+        <v>0.86080000000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="74" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" t="b">
+        <v>1</v>
+      </c>
+      <c r="B74">
+        <v>35</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" t="b">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0.873</v>
+      </c>
+      <c r="I74">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="J74">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="K74">
+        <v>0.84199999999999997</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" t="b">
+        <v>1</v>
+      </c>
+      <c r="B75">
+        <v>35</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" t="b">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0.874</v>
+      </c>
+      <c r="I75">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="J75">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="K75">
+        <v>0.85199999999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" t="b">
+        <v>1</v>
+      </c>
+      <c r="B76">
+        <v>35</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" t="b">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0.89</v>
+      </c>
+      <c r="I76">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="J76">
+        <v>0.872</v>
+      </c>
+      <c r="K76">
+        <v>0.88900000000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" t="b">
+        <v>1</v>
+      </c>
+      <c r="B77">
+        <v>35</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" t="b">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="I77">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="J77">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="K77">
+        <v>0.91300000000000003</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" t="b">
+        <v>1</v>
+      </c>
+      <c r="B78">
+        <v>35</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78" t="b">
+        <v>0</v>
+      </c>
+      <c r="E78" t="b">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="I78">
+        <v>0.83</v>
+      </c>
+      <c r="J78">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="K78">
+        <v>0.77900000000000003</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" t="b">
+        <v>1</v>
+      </c>
+      <c r="B79">
+        <v>35</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79" t="b">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="I79">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="J79">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="K79">
+        <v>0.88300000000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="H80">
+        <f>AVERAGE(H74:H79)</f>
+        <v>0.86900000000000011</v>
+      </c>
+      <c r="I80">
+        <f t="shared" ref="I80:K80" si="9">AVERAGE(I74:I79)</f>
+        <v>0.84666666666666657</v>
+      </c>
+      <c r="J80">
+        <f t="shared" si="9"/>
+        <v>0.86950000000000005</v>
+      </c>
+      <c r="K80">
+        <f t="shared" si="9"/>
+        <v>0.85966666666666669</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" t="b">
+        <v>1</v>
+      </c>
+      <c r="B83">
+        <v>37</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" t="b">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="I83">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="J83">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="K83">
+        <v>0.90100000000000002</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" t="b">
+        <v>1</v>
+      </c>
+      <c r="B84">
+        <v>37</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" t="b">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="I84">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="J84">
+        <v>0.81</v>
+      </c>
+      <c r="K84">
+        <v>0.89100000000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" t="b">
+        <v>1</v>
+      </c>
+      <c r="B85">
+        <v>37</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85" t="b">
+        <v>0</v>
+      </c>
+      <c r="E85" t="b">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>0.86</v>
+      </c>
+      <c r="I85">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="J85">
+        <v>0.86</v>
+      </c>
+      <c r="K85">
+        <v>0.86099999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" t="b">
+        <v>1</v>
+      </c>
+      <c r="B86">
+        <v>37</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86" t="b">
+        <v>0</v>
+      </c>
+      <c r="E86" t="b">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="I86">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="J86">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="K86">
+        <v>0.88800000000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" t="b">
+        <v>1</v>
+      </c>
+      <c r="B87">
+        <v>37</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" t="b">
+        <v>0</v>
+      </c>
+      <c r="I87" s="2"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="H88">
+        <f>AVERAGE(H83:H87)</f>
+        <v>0.86224999999999996</v>
+      </c>
+      <c r="I88">
+        <f t="shared" ref="I88:J88" si="10">AVERAGE(I83:I87)</f>
+        <v>0.84525000000000006</v>
+      </c>
+      <c r="J88">
+        <f t="shared" si="10"/>
+        <v>0.83174999999999999</v>
+      </c>
+      <c r="K88">
+        <f>AVERAGE(K83:K87)</f>
+        <v>0.88524999999999998</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1</v>
+      </c>
+      <c r="C91" t="s">
+        <v>2</v>
+      </c>
+      <c r="D91" t="s">
+        <v>3</v>
+      </c>
+      <c r="E91" t="s">
+        <v>14</v>
+      </c>
+      <c r="H91" t="s">
+        <v>4</v>
+      </c>
+      <c r="I91" t="s">
+        <v>5</v>
+      </c>
+      <c r="J91" t="s">
+        <v>6</v>
+      </c>
+      <c r="K91" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" t="b">
+        <v>1</v>
+      </c>
+      <c r="B92">
+        <v>31</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" t="b">
+        <v>1</v>
+      </c>
+      <c r="H92">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="I92">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="J92">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="K92">
+        <v>0.86599999999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" t="b">
+        <v>1</v>
+      </c>
+      <c r="B93">
+        <v>31</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" t="b">
+        <v>1</v>
+      </c>
+      <c r="H93">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="I93">
+        <v>0.85</v>
+      </c>
+      <c r="J93">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="K93">
+        <v>0.89500000000000002</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" t="b">
+        <v>1</v>
+      </c>
+      <c r="B94">
+        <v>31</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94" t="b">
+        <v>0</v>
+      </c>
+      <c r="E94" t="b">
+        <v>1</v>
+      </c>
+      <c r="H94">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="I94">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="J94">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="K94">
+        <v>0.86699999999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" t="b">
+        <v>1</v>
+      </c>
+      <c r="B95">
+        <v>31</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95" t="b">
+        <v>0</v>
+      </c>
+      <c r="E95" t="b">
+        <v>1</v>
+      </c>
+      <c r="H95">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="I95">
+        <v>0.85</v>
+      </c>
+      <c r="J95">
+        <v>0.9</v>
+      </c>
+      <c r="K95">
+        <v>0.85399999999999998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" t="b">
+        <v>1</v>
+      </c>
+      <c r="B96">
+        <v>31</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96" t="b">
+        <v>0</v>
+      </c>
+      <c r="E96" t="b">
+        <v>1</v>
+      </c>
+      <c r="H96">
+        <v>0.9</v>
+      </c>
+      <c r="I96">
+        <v>0.86</v>
+      </c>
+      <c r="J96">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="K96">
+        <v>0.873</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" t="b">
+        <v>1</v>
+      </c>
+      <c r="B97">
+        <v>31</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97" t="b">
+        <v>1</v>
+      </c>
+      <c r="H97">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="I97">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="J97">
+        <v>0.877</v>
+      </c>
+      <c r="K97">
+        <v>0.873</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" t="b">
+        <v>1</v>
+      </c>
+      <c r="B98">
+        <v>31</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98" t="b">
+        <v>0</v>
+      </c>
+      <c r="E98" t="b">
+        <v>1</v>
+      </c>
+      <c r="H98">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="I98">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="J98">
         <v>0.82</v>
       </c>
-      <c r="K67">
+      <c r="K98">
         <v>0.89600000000000002</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H68">
-        <f>AVERAGE(H61:H67)</f>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="H99">
+        <f>AVERAGE(H92:H98)</f>
         <v>0.89171428571428568</v>
       </c>
-      <c r="I68">
-        <f t="shared" ref="I68:K68" si="8">AVERAGE(I61:I67)</f>
+      <c r="I99">
+        <f t="shared" ref="I99:K99" si="11">AVERAGE(I92:I98)</f>
         <v>0.84957142857142876</v>
       </c>
-      <c r="J68">
-        <f t="shared" si="8"/>
+      <c r="J99">
+        <f t="shared" si="11"/>
         <v>0.89171428571428568</v>
       </c>
-      <c r="K68">
-        <f t="shared" si="8"/>
+      <c r="K99">
+        <f t="shared" si="11"/>
         <v>0.87485714285714289</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" t="s">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" t="s">
-        <v>0</v>
-      </c>
-      <c r="B72" t="s">
-        <v>1</v>
-      </c>
-      <c r="C72" t="s">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" t="s">
+        <v>0</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" t="s">
         <v>2</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D103" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" t="b">
-        <v>1</v>
-      </c>
-      <c r="B73">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" t="b">
+        <v>1</v>
+      </c>
+      <c r="B104">
         <v>21</v>
       </c>
-      <c r="C73">
-        <v>0</v>
-      </c>
-      <c r="D73" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" t="b">
-        <v>1</v>
-      </c>
-      <c r="B74">
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" t="b">
+        <v>1</v>
+      </c>
+      <c r="B105">
         <v>21</v>
       </c>
-      <c r="C74">
-        <v>0</v>
-      </c>
-      <c r="D74" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" t="b">
-        <v>1</v>
-      </c>
-      <c r="B75">
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="D105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" t="b">
+        <v>1</v>
+      </c>
+      <c r="B106">
         <v>21</v>
       </c>
-      <c r="C75">
-        <v>0</v>
-      </c>
-      <c r="D75" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" t="b">
-        <v>1</v>
-      </c>
-      <c r="B76">
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" t="b">
+        <v>1</v>
+      </c>
+      <c r="B107">
         <v>21</v>
       </c>
-      <c r="C76">
-        <v>0</v>
-      </c>
-      <c r="D76" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A77" t="b">
-        <v>1</v>
-      </c>
-      <c r="B77">
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" t="b">
+        <v>1</v>
+      </c>
+      <c r="B108">
         <v>21</v>
       </c>
-      <c r="C77">
-        <v>0</v>
-      </c>
-      <c r="D77" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A78" t="b">
-        <v>1</v>
-      </c>
-      <c r="B78">
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" t="b">
+        <v>1</v>
+      </c>
+      <c r="B109">
         <v>21</v>
       </c>
-      <c r="C78">
-        <v>0</v>
-      </c>
-      <c r="D78" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A79" t="b">
-        <v>1</v>
-      </c>
-      <c r="B79">
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="D109" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" t="b">
+        <v>1</v>
+      </c>
+      <c r="B110">
         <v>21</v>
       </c>
-      <c r="C79">
-        <v>0</v>
-      </c>
-      <c r="D79" t="b">
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix an out of bounds error when changing the number of frames
</commit_message>
<xml_diff>
--- a/evaluation/training-evaluation.xlsx
+++ b/evaluation/training-evaluation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - University of Cyprus\ucl\thesis\workspace\cell-tracking-ucl-thesis\evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8F5600-FAA6-4EF1-810D-025292F001D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73192E4B-C619-455A-9D64-EED6567B6ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{DD5E1588-BB96-47E2-8F58-F1B1A8926599}"/>
   </bookViews>
@@ -87,7 +87,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,12 +102,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="4"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -130,12 +124,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25252485-713D-4CC8-BE64-95040359BD5A}">
-  <dimension ref="A1:K110"/>
+  <dimension ref="A1:K135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="P77" sqref="P77"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="N101" sqref="N101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1757,16 +1748,16 @@
         <v>0</v>
       </c>
       <c r="H67">
-        <v>0.89</v>
+        <v>0.86199999999999999</v>
       </c>
       <c r="I67">
-        <v>0.84399999999999997</v>
+        <v>0.84799999999999998</v>
       </c>
       <c r="J67">
-        <v>0.92700000000000005</v>
+        <v>0.83899999999999997</v>
       </c>
       <c r="K67">
-        <v>0.83499999999999996</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1786,16 +1777,16 @@
         <v>0</v>
       </c>
       <c r="H68">
-        <v>0.88300000000000001</v>
+        <v>0.877</v>
       </c>
       <c r="I68">
-        <v>0.84</v>
+        <v>0.84399999999999997</v>
       </c>
       <c r="J68">
-        <v>0.89800000000000002</v>
+        <v>0.90100000000000002</v>
       </c>
       <c r="K68">
-        <v>0.85199999999999998</v>
+        <v>0.84099999999999997</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1815,16 +1806,16 @@
         <v>0</v>
       </c>
       <c r="H69">
-        <v>0.86499999999999999</v>
+        <v>0.83499999999999996</v>
       </c>
       <c r="I69">
-        <v>0.83399999999999996</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="J69">
-        <v>0.86799999999999999</v>
+        <v>0.81299999999999994</v>
       </c>
       <c r="K69">
-        <v>0.85</v>
+        <v>0.85199999999999998</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1844,16 +1835,16 @@
         <v>0</v>
       </c>
       <c r="H70">
-        <v>0.878</v>
+        <v>0.88300000000000001</v>
       </c>
       <c r="I70">
-        <v>0.84299999999999997</v>
+        <v>0.84899999999999998</v>
       </c>
       <c r="J70">
-        <v>0.85</v>
+        <v>0.90700000000000003</v>
       </c>
       <c r="K70">
-        <v>0.89200000000000002</v>
+        <v>0.84599999999999997</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1873,182 +1864,182 @@
         <v>0</v>
       </c>
       <c r="H71">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="I71">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="J71">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="K71">
+        <v>0.88200000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" t="b">
+        <v>1</v>
+      </c>
+      <c r="B72">
+        <v>31</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" t="b">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0.89</v>
+      </c>
+      <c r="I72">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="J72">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="K72">
+        <v>0.83499999999999996</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" t="b">
+        <v>1</v>
+      </c>
+      <c r="B73">
+        <v>31</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" t="b">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="I73">
+        <v>0.84</v>
+      </c>
+      <c r="J73">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="K73">
+        <v>0.85199999999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" t="b">
+        <v>1</v>
+      </c>
+      <c r="B74">
+        <v>31</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" t="b">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="I74">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="J74">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="K74">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" t="b">
+        <v>1</v>
+      </c>
+      <c r="B75">
+        <v>31</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" t="b">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0.878</v>
+      </c>
+      <c r="I75">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="J75">
+        <v>0.85</v>
+      </c>
+      <c r="K75">
+        <v>0.89200000000000002</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" t="b">
+        <v>1</v>
+      </c>
+      <c r="B76">
+        <v>31</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" t="b">
+        <v>0</v>
+      </c>
+      <c r="H76">
         <v>0.85699999999999998</v>
       </c>
-      <c r="I71">
+      <c r="I76">
         <v>0.83399999999999996</v>
       </c>
-      <c r="J71">
+      <c r="J76">
         <v>0.82899999999999996</v>
       </c>
-      <c r="K71">
+      <c r="K76">
         <v>0.875</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="H72">
-        <f>AVERAGE(H67:H71)</f>
-        <v>0.87460000000000004</v>
-      </c>
-      <c r="I72">
-        <f t="shared" ref="I72:K72" si="8">AVERAGE(I67:I71)</f>
-        <v>0.83899999999999986</v>
-      </c>
-      <c r="J72">
+    <row r="77" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="H77">
+        <f t="shared" ref="H77:J77" si="8">AVERAGE(H67:H76)</f>
+        <v>0.86820000000000008</v>
+      </c>
+      <c r="I77">
         <f t="shared" si="8"/>
-        <v>0.87439999999999996</v>
-      </c>
-      <c r="K72">
+        <v>0.83979999999999999</v>
+      </c>
+      <c r="J77">
         <f t="shared" si="8"/>
-        <v>0.86080000000000001</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="74" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" t="b">
-        <v>1</v>
-      </c>
-      <c r="B74">
-        <v>35</v>
-      </c>
-      <c r="C74">
-        <v>0</v>
-      </c>
-      <c r="D74" t="b">
-        <v>0</v>
-      </c>
-      <c r="E74" t="b">
-        <v>0</v>
-      </c>
-      <c r="H74">
-        <v>0.873</v>
-      </c>
-      <c r="I74">
-        <v>0.85499999999999998</v>
-      </c>
-      <c r="J74">
-        <v>0.89800000000000002</v>
-      </c>
-      <c r="K74">
-        <v>0.84199999999999997</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" t="b">
-        <v>1</v>
-      </c>
-      <c r="B75">
-        <v>35</v>
-      </c>
-      <c r="C75">
-        <v>0</v>
-      </c>
-      <c r="D75" t="b">
-        <v>0</v>
-      </c>
-      <c r="E75" t="b">
-        <v>0</v>
-      </c>
-      <c r="H75">
-        <v>0.874</v>
-      </c>
-      <c r="I75">
-        <v>0.85499999999999998</v>
-      </c>
-      <c r="J75">
-        <v>0.88900000000000001</v>
-      </c>
-      <c r="K75">
-        <v>0.85199999999999998</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" t="b">
-        <v>1</v>
-      </c>
-      <c r="B76">
-        <v>35</v>
-      </c>
-      <c r="C76">
-        <v>0</v>
-      </c>
-      <c r="D76" t="b">
-        <v>0</v>
-      </c>
-      <c r="E76" t="b">
-        <v>0</v>
-      </c>
-      <c r="H76">
-        <v>0.89</v>
-      </c>
-      <c r="I76">
-        <v>0.84399999999999997</v>
-      </c>
-      <c r="J76">
-        <v>0.872</v>
-      </c>
-      <c r="K76">
-        <v>0.88900000000000001</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A77" t="b">
-        <v>1</v>
-      </c>
-      <c r="B77">
-        <v>35</v>
-      </c>
-      <c r="C77">
-        <v>0</v>
-      </c>
-      <c r="D77" t="b">
-        <v>0</v>
-      </c>
-      <c r="E77" t="b">
-        <v>0</v>
-      </c>
-      <c r="H77">
-        <v>0.86399999999999999</v>
-      </c>
-      <c r="I77">
-        <v>0.85099999999999998</v>
-      </c>
-      <c r="J77">
-        <v>0.80900000000000005</v>
+        <v>0.86470000000000002</v>
       </c>
       <c r="K77">
-        <v>0.91300000000000003</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A78" t="b">
-        <v>1</v>
-      </c>
-      <c r="B78">
-        <v>35</v>
-      </c>
-      <c r="C78">
-        <v>0</v>
-      </c>
-      <c r="D78" t="b">
-        <v>0</v>
-      </c>
-      <c r="E78" t="b">
-        <v>0</v>
-      </c>
-      <c r="H78">
-        <v>0.85099999999999998</v>
-      </c>
-      <c r="I78">
-        <v>0.83</v>
-      </c>
-      <c r="J78">
-        <v>0.91600000000000004</v>
-      </c>
-      <c r="K78">
-        <v>0.77900000000000003</v>
-      </c>
-    </row>
+        <f>AVERAGE(K67:K76)</f>
+        <v>0.86050000000000004</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="79" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="b">
         <v>1</v>
@@ -2066,153 +2057,182 @@
         <v>0</v>
       </c>
       <c r="H79">
+        <v>0.873</v>
+      </c>
+      <c r="I79">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="J79">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="K79">
+        <v>0.84199999999999997</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" t="b">
+        <v>1</v>
+      </c>
+      <c r="B80">
+        <v>35</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80" t="b">
+        <v>0</v>
+      </c>
+      <c r="E80" t="b">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>0.874</v>
+      </c>
+      <c r="I80">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="J80">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="K80">
+        <v>0.85199999999999998</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" t="b">
+        <v>1</v>
+      </c>
+      <c r="B81">
+        <v>35</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81" t="b">
+        <v>0</v>
+      </c>
+      <c r="E81" t="b">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0.89</v>
+      </c>
+      <c r="I81">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="J81">
+        <v>0.872</v>
+      </c>
+      <c r="K81">
+        <v>0.88900000000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" t="b">
+        <v>1</v>
+      </c>
+      <c r="B82">
+        <v>35</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" t="b">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="I82">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="J82">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="K82">
+        <v>0.91300000000000003</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" t="b">
+        <v>1</v>
+      </c>
+      <c r="B83">
+        <v>35</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" t="b">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="I83">
+        <v>0.83</v>
+      </c>
+      <c r="J83">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="K83">
+        <v>0.77900000000000003</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" t="b">
+        <v>1</v>
+      </c>
+      <c r="B84">
+        <v>35</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" t="b">
+        <v>0</v>
+      </c>
+      <c r="H84">
         <v>0.86199999999999999</v>
       </c>
-      <c r="I79">
+      <c r="I84">
         <v>0.84499999999999997</v>
       </c>
-      <c r="J79">
+      <c r="J84">
         <v>0.83299999999999996</v>
       </c>
-      <c r="K79">
+      <c r="K84">
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="H80">
-        <f>AVERAGE(H74:H79)</f>
+    <row r="85" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="H85">
+        <f>AVERAGE(H79:H84)</f>
         <v>0.86900000000000011</v>
       </c>
-      <c r="I80">
-        <f t="shared" ref="I80:K80" si="9">AVERAGE(I74:I79)</f>
+      <c r="I85">
+        <f t="shared" ref="I85:K85" si="9">AVERAGE(I79:I84)</f>
         <v>0.84666666666666657</v>
       </c>
-      <c r="J80">
+      <c r="J85">
         <f t="shared" si="9"/>
         <v>0.86950000000000005</v>
       </c>
-      <c r="K80">
+      <c r="K85">
         <f t="shared" si="9"/>
         <v>0.85966666666666669</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A83" t="b">
-        <v>1</v>
-      </c>
-      <c r="B83">
-        <v>37</v>
-      </c>
-      <c r="C83">
-        <v>0</v>
-      </c>
-      <c r="D83" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" t="b">
-        <v>0</v>
-      </c>
-      <c r="H83">
-        <v>0.86299999999999999</v>
-      </c>
-      <c r="I83">
-        <v>0.83899999999999997</v>
-      </c>
-      <c r="J83">
-        <v>0.81499999999999995</v>
-      </c>
-      <c r="K83">
-        <v>0.90100000000000002</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84" t="b">
-        <v>1</v>
-      </c>
-      <c r="B84">
-        <v>37</v>
-      </c>
-      <c r="C84">
-        <v>0</v>
-      </c>
-      <c r="D84" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" t="b">
-        <v>0</v>
-      </c>
-      <c r="H84">
-        <v>0.85699999999999998</v>
-      </c>
-      <c r="I84">
-        <v>0.82899999999999996</v>
-      </c>
-      <c r="J84">
-        <v>0.81</v>
-      </c>
-      <c r="K84">
-        <v>0.89100000000000001</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" t="b">
-        <v>1</v>
-      </c>
-      <c r="B85">
-        <v>37</v>
-      </c>
-      <c r="C85">
-        <v>0</v>
-      </c>
-      <c r="D85" t="b">
-        <v>0</v>
-      </c>
-      <c r="E85" t="b">
-        <v>0</v>
-      </c>
-      <c r="H85">
-        <v>0.86</v>
-      </c>
-      <c r="I85">
-        <v>0.86399999999999999</v>
-      </c>
-      <c r="J85">
-        <v>0.86</v>
-      </c>
-      <c r="K85">
-        <v>0.86099999999999999</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86" t="b">
-        <v>1</v>
-      </c>
-      <c r="B86">
-        <v>37</v>
-      </c>
-      <c r="C86">
-        <v>0</v>
-      </c>
-      <c r="D86" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" t="b">
-        <v>0</v>
-      </c>
-      <c r="H86">
-        <v>0.86899999999999999</v>
-      </c>
-      <c r="I86">
-        <v>0.84899999999999998</v>
-      </c>
-      <c r="J86">
-        <v>0.84199999999999997</v>
-      </c>
-      <c r="K86">
-        <v>0.88800000000000001</v>
-      </c>
-    </row>
+    <row r="86" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="87" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="b">
         <v>1</v>
@@ -2229,87 +2249,122 @@
       <c r="E87" t="b">
         <v>0</v>
       </c>
-      <c r="I87" s="2"/>
+      <c r="H87">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="I87">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="J87">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="K87">
+        <v>0.90100000000000002</v>
+      </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" t="b">
+        <v>1</v>
+      </c>
+      <c r="B88">
+        <v>37</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" t="b">
+        <v>0</v>
+      </c>
       <c r="H88">
-        <f>AVERAGE(H83:H87)</f>
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="I88">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="J88">
+        <v>0.81</v>
+      </c>
+      <c r="K88">
+        <v>0.89100000000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" t="b">
+        <v>1</v>
+      </c>
+      <c r="B89">
+        <v>37</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" t="b">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>0.86</v>
+      </c>
+      <c r="I89">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="J89">
+        <v>0.86</v>
+      </c>
+      <c r="K89">
+        <v>0.86099999999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" t="b">
+        <v>1</v>
+      </c>
+      <c r="B90">
+        <v>37</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" t="b">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="I90">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="J90">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="K90">
+        <v>0.88800000000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="H91">
+        <f>AVERAGE(H87:H90)</f>
         <v>0.86224999999999996</v>
       </c>
-      <c r="I88">
-        <f t="shared" ref="I88:J88" si="10">AVERAGE(I83:I87)</f>
+      <c r="I91">
+        <f>AVERAGE(I87:I90)</f>
         <v>0.84525000000000006</v>
       </c>
-      <c r="J88">
-        <f t="shared" si="10"/>
+      <c r="J91">
+        <f>AVERAGE(J87:J90)</f>
         <v>0.83174999999999999</v>
       </c>
-      <c r="K88">
-        <f>AVERAGE(K83:K87)</f>
+      <c r="K91">
+        <f>AVERAGE(K87:K90)</f>
         <v>0.88524999999999998</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A90" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A91" t="s">
-        <v>0</v>
-      </c>
-      <c r="B91" t="s">
-        <v>1</v>
-      </c>
-      <c r="C91" t="s">
-        <v>2</v>
-      </c>
-      <c r="D91" t="s">
-        <v>3</v>
-      </c>
-      <c r="E91" t="s">
-        <v>14</v>
-      </c>
-      <c r="H91" t="s">
-        <v>4</v>
-      </c>
-      <c r="I91" t="s">
-        <v>5</v>
-      </c>
-      <c r="J91" t="s">
-        <v>6</v>
-      </c>
-      <c r="K91" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A92" t="b">
-        <v>1</v>
-      </c>
-      <c r="B92">
-        <v>31</v>
-      </c>
-      <c r="C92">
-        <v>0</v>
-      </c>
-      <c r="D92" t="b">
-        <v>0</v>
-      </c>
-      <c r="E92" t="b">
-        <v>1</v>
-      </c>
-      <c r="H92">
-        <v>0.90300000000000002</v>
-      </c>
-      <c r="I92">
-        <v>0.84699999999999998</v>
-      </c>
-      <c r="J92">
-        <v>0.91800000000000004</v>
-      </c>
-      <c r="K92">
-        <v>0.86599999999999999</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2317,7 +2372,7 @@
         <v>1</v>
       </c>
       <c r="B93">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -2326,19 +2381,19 @@
         <v>0</v>
       </c>
       <c r="E93" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H93">
-        <v>0.92500000000000004</v>
+        <v>0.875</v>
       </c>
       <c r="I93">
-        <v>0.85</v>
+        <v>0.84899999999999998</v>
       </c>
       <c r="J93">
-        <v>0.92400000000000004</v>
+        <v>0.84</v>
       </c>
       <c r="K93">
-        <v>0.89500000000000002</v>
+        <v>0.89900000000000002</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2346,7 +2401,7 @@
         <v>1</v>
       </c>
       <c r="B94">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -2355,19 +2410,19 @@
         <v>0</v>
       </c>
       <c r="E94" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H94">
         <v>0.88600000000000001</v>
       </c>
       <c r="I94">
-        <v>0.85199999999999998</v>
+        <v>0.86</v>
       </c>
       <c r="J94">
-        <v>0.89200000000000002</v>
+        <v>0.86</v>
       </c>
       <c r="K94">
-        <v>0.86699999999999999</v>
+        <v>0.90100000000000002</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2375,7 +2430,7 @@
         <v>1</v>
       </c>
       <c r="B95">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -2384,19 +2439,19 @@
         <v>0</v>
       </c>
       <c r="E95" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H95">
-        <v>0.88400000000000001</v>
+        <v>0.86799999999999999</v>
       </c>
       <c r="I95">
-        <v>0.85</v>
+        <v>0.85499999999999998</v>
       </c>
       <c r="J95">
-        <v>0.9</v>
+        <v>0.87</v>
       </c>
       <c r="K95">
-        <v>0.85399999999999998</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2404,7 +2459,7 @@
         <v>1</v>
       </c>
       <c r="B96">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -2413,19 +2468,19 @@
         <v>0</v>
       </c>
       <c r="E96" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H96">
-        <v>0.9</v>
+        <v>0.90900000000000003</v>
       </c>
       <c r="I96">
-        <v>0.86</v>
+        <v>0.85299999999999998</v>
       </c>
       <c r="J96">
-        <v>0.91100000000000003</v>
+        <v>0.88700000000000001</v>
       </c>
       <c r="K96">
-        <v>0.873</v>
+        <v>0.90800000000000003</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2433,7 +2488,7 @@
         <v>1</v>
       </c>
       <c r="B97">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -2442,85 +2497,153 @@
         <v>0</v>
       </c>
       <c r="E97" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H97">
-        <v>0.88300000000000001</v>
+        <v>0.88200000000000001</v>
       </c>
       <c r="I97">
-        <v>0.84399999999999997</v>
+        <v>0.83699999999999997</v>
       </c>
       <c r="J97">
-        <v>0.877</v>
+        <v>0.81200000000000006</v>
       </c>
       <c r="K97">
-        <v>0.873</v>
+        <v>0.93200000000000005</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" t="b">
-        <v>1</v>
-      </c>
-      <c r="B98">
-        <v>31</v>
-      </c>
-      <c r="C98">
-        <v>0</v>
-      </c>
-      <c r="D98" t="b">
-        <v>0</v>
-      </c>
-      <c r="E98" t="b">
-        <v>1</v>
-      </c>
       <c r="H98">
-        <v>0.86099999999999999</v>
+        <f>AVERAGE(H87:H97)</f>
+        <v>0.87312499999999993</v>
       </c>
       <c r="I98">
-        <v>0.84399999999999997</v>
+        <f>AVERAGE(I87:I97)</f>
+        <v>0.84802500000000003</v>
       </c>
       <c r="J98">
-        <v>0.82</v>
+        <f>AVERAGE(J87:J97)</f>
+        <v>0.84277499999999994</v>
       </c>
       <c r="K98">
-        <v>0.89600000000000002</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="H99">
-        <f>AVERAGE(H92:H98)</f>
-        <v>0.89171428571428568</v>
-      </c>
-      <c r="I99">
-        <f t="shared" ref="I99:K99" si="11">AVERAGE(I92:I98)</f>
-        <v>0.84957142857142876</v>
-      </c>
-      <c r="J99">
-        <f t="shared" si="11"/>
-        <v>0.89171428571428568</v>
-      </c>
-      <c r="K99">
-        <f t="shared" si="11"/>
-        <v>0.87485714285714289</v>
+        <f>AVERAGE(K87:K97)</f>
+        <v>0.892625</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" t="b">
+        <v>1</v>
+      </c>
+      <c r="B100">
+        <v>45</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100" t="b">
+        <v>0</v>
+      </c>
+      <c r="E100" t="b">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="I100">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="J100">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="K100">
+        <v>0.91200000000000003</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" t="b">
+        <v>1</v>
+      </c>
+      <c r="B101">
+        <v>45</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101" t="b">
+        <v>0</v>
+      </c>
+      <c r="E101" t="b">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="I101">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="J101">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="K101">
+        <v>0.88400000000000001</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A102" t="s">
-        <v>13</v>
+      <c r="A102" t="b">
+        <v>1</v>
+      </c>
+      <c r="B102">
+        <v>45</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102" t="b">
+        <v>0</v>
+      </c>
+      <c r="E102" t="b">
+        <v>0</v>
+      </c>
+      <c r="H102">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="I102">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="J102">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="K102">
+        <v>0.90700000000000003</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A103" t="s">
-        <v>0</v>
-      </c>
-      <c r="B103" t="s">
-        <v>1</v>
-      </c>
-      <c r="C103" t="s">
-        <v>2</v>
-      </c>
-      <c r="D103" t="s">
-        <v>3</v>
+      <c r="A103" t="b">
+        <v>1</v>
+      </c>
+      <c r="B103">
+        <v>45</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103" t="b">
+        <v>0</v>
+      </c>
+      <c r="E103" t="b">
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="I103">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="J103">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="K103">
+        <v>0.86699999999999999</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2528,96 +2651,417 @@
         <v>1</v>
       </c>
       <c r="B104">
+        <v>45</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104" t="b">
+        <v>0</v>
+      </c>
+      <c r="E104" t="b">
+        <v>0</v>
+      </c>
+      <c r="H104">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="I104">
+        <v>0.86</v>
+      </c>
+      <c r="J104">
+        <v>0.879</v>
+      </c>
+      <c r="K104">
+        <v>0.879</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="H105">
+        <f>AVERAGE(H93:H103)</f>
+        <v>0.8899125</v>
+      </c>
+      <c r="I105">
+        <f>AVERAGE(I93:I103)</f>
+        <v>0.85510249999999988</v>
+      </c>
+      <c r="J105">
+        <f>AVERAGE(J93:J103)</f>
+        <v>0.86907750000000006</v>
+      </c>
+      <c r="K105">
+        <f>AVERAGE(K93:K103)</f>
+        <v>0.89626249999999996</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116" t="s">
+        <v>0</v>
+      </c>
+      <c r="B116" t="s">
+        <v>1</v>
+      </c>
+      <c r="C116" t="s">
+        <v>2</v>
+      </c>
+      <c r="D116" t="s">
+        <v>3</v>
+      </c>
+      <c r="E116" t="s">
+        <v>14</v>
+      </c>
+      <c r="H116" t="s">
+        <v>4</v>
+      </c>
+      <c r="I116" t="s">
+        <v>5</v>
+      </c>
+      <c r="J116" t="s">
+        <v>6</v>
+      </c>
+      <c r="K116" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" t="b">
+        <v>1</v>
+      </c>
+      <c r="B117">
+        <v>31</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
+      <c r="D117" t="b">
+        <v>0</v>
+      </c>
+      <c r="E117" t="b">
+        <v>1</v>
+      </c>
+      <c r="H117">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="I117">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="J117">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="K117">
+        <v>0.86599999999999999</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118" t="b">
+        <v>1</v>
+      </c>
+      <c r="B118">
+        <v>31</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+      <c r="D118" t="b">
+        <v>0</v>
+      </c>
+      <c r="E118" t="b">
+        <v>1</v>
+      </c>
+      <c r="H118">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="I118">
+        <v>0.85</v>
+      </c>
+      <c r="J118">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="K118">
+        <v>0.89500000000000002</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119" t="b">
+        <v>1</v>
+      </c>
+      <c r="B119">
+        <v>31</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+      <c r="D119" t="b">
+        <v>0</v>
+      </c>
+      <c r="E119" t="b">
+        <v>1</v>
+      </c>
+      <c r="H119">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="I119">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="J119">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="K119">
+        <v>0.86699999999999999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120" t="b">
+        <v>1</v>
+      </c>
+      <c r="B120">
+        <v>31</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120" t="b">
+        <v>0</v>
+      </c>
+      <c r="E120" t="b">
+        <v>1</v>
+      </c>
+      <c r="H120">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="I120">
+        <v>0.85</v>
+      </c>
+      <c r="J120">
+        <v>0.9</v>
+      </c>
+      <c r="K120">
+        <v>0.85399999999999998</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121" t="b">
+        <v>1</v>
+      </c>
+      <c r="B121">
+        <v>31</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
+      <c r="D121" t="b">
+        <v>0</v>
+      </c>
+      <c r="E121" t="b">
+        <v>1</v>
+      </c>
+      <c r="H121">
+        <v>0.9</v>
+      </c>
+      <c r="I121">
+        <v>0.86</v>
+      </c>
+      <c r="J121">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="K121">
+        <v>0.873</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122" t="b">
+        <v>1</v>
+      </c>
+      <c r="B122">
+        <v>31</v>
+      </c>
+      <c r="C122">
+        <v>0</v>
+      </c>
+      <c r="D122" t="b">
+        <v>0</v>
+      </c>
+      <c r="E122" t="b">
+        <v>1</v>
+      </c>
+      <c r="H122">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="I122">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="J122">
+        <v>0.877</v>
+      </c>
+      <c r="K122">
+        <v>0.873</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123" t="b">
+        <v>1</v>
+      </c>
+      <c r="B123">
+        <v>31</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+      <c r="D123" t="b">
+        <v>0</v>
+      </c>
+      <c r="E123" t="b">
+        <v>1</v>
+      </c>
+      <c r="H123">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="I123">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="J123">
+        <v>0.82</v>
+      </c>
+      <c r="K123">
+        <v>0.89600000000000002</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="H124">
+        <f>AVERAGE(H117:H123)</f>
+        <v>0.89171428571428568</v>
+      </c>
+      <c r="I124">
+        <f t="shared" ref="I124:K124" si="10">AVERAGE(I117:I123)</f>
+        <v>0.84957142857142876</v>
+      </c>
+      <c r="J124">
+        <f t="shared" si="10"/>
+        <v>0.89171428571428568</v>
+      </c>
+      <c r="K124">
+        <f t="shared" si="10"/>
+        <v>0.87485714285714289</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128" t="s">
+        <v>0</v>
+      </c>
+      <c r="B128" t="s">
+        <v>1</v>
+      </c>
+      <c r="C128" t="s">
+        <v>2</v>
+      </c>
+      <c r="D128" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129" t="b">
+        <v>1</v>
+      </c>
+      <c r="B129">
         <v>21</v>
       </c>
-      <c r="C104">
-        <v>0</v>
-      </c>
-      <c r="D104" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A105" t="b">
-        <v>1</v>
-      </c>
-      <c r="B105">
+      <c r="C129">
+        <v>0</v>
+      </c>
+      <c r="D129" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130" t="b">
+        <v>1</v>
+      </c>
+      <c r="B130">
         <v>21</v>
       </c>
-      <c r="C105">
-        <v>0</v>
-      </c>
-      <c r="D105" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A106" t="b">
-        <v>1</v>
-      </c>
-      <c r="B106">
+      <c r="C130">
+        <v>0</v>
+      </c>
+      <c r="D130" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131" t="b">
+        <v>1</v>
+      </c>
+      <c r="B131">
         <v>21</v>
       </c>
-      <c r="C106">
-        <v>0</v>
-      </c>
-      <c r="D106" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A107" t="b">
-        <v>1</v>
-      </c>
-      <c r="B107">
+      <c r="C131">
+        <v>0</v>
+      </c>
+      <c r="D131" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" t="b">
+        <v>1</v>
+      </c>
+      <c r="B132">
         <v>21</v>
       </c>
-      <c r="C107">
-        <v>0</v>
-      </c>
-      <c r="D107" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A108" t="b">
-        <v>1</v>
-      </c>
-      <c r="B108">
+      <c r="C132">
+        <v>0</v>
+      </c>
+      <c r="D132" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" t="b">
+        <v>1</v>
+      </c>
+      <c r="B133">
         <v>21</v>
       </c>
-      <c r="C108">
-        <v>0</v>
-      </c>
-      <c r="D108" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A109" t="b">
-        <v>1</v>
-      </c>
-      <c r="B109">
+      <c r="C133">
+        <v>0</v>
+      </c>
+      <c r="D133" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134" t="b">
+        <v>1</v>
+      </c>
+      <c r="B134">
         <v>21</v>
       </c>
-      <c r="C109">
-        <v>0</v>
-      </c>
-      <c r="D109" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A110" t="b">
-        <v>1</v>
-      </c>
-      <c r="B110">
+      <c r="C134">
+        <v>0</v>
+      </c>
+      <c r="D134" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135" t="b">
+        <v>1</v>
+      </c>
+      <c r="B135">
         <v>21</v>
       </c>
-      <c r="C110">
-        <v>0</v>
-      </c>
-      <c r="D110" t="b">
+      <c r="C135">
+        <v>0</v>
+      </c>
+      <c r="D135" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made patch extraction radius different from patch size so that the negatives are close to the positives because higher patch sizes used to give higher accuracy because they were further away
</commit_message>
<xml_diff>
--- a/evaluation/training-evaluation.xlsx
+++ b/evaluation/training-evaluation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - University of Cyprus\ucl\thesis\workspace\cell-tracking-ucl-thesis\evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73192E4B-C619-455A-9D64-EED6567B6ACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C618D407-C022-4163-8972-D53B2D3E9624}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{DD5E1588-BB96-47E2-8F58-F1B1A8926599}"/>
   </bookViews>
@@ -443,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25252485-713D-4CC8-BE64-95040359BD5A}">
   <dimension ref="A1:K135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="N101" sqref="N101"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="N111" sqref="N111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2693,6 +2693,151 @@
         <v>0.89626249999999996</v>
       </c>
     </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" t="b">
+        <v>1</v>
+      </c>
+      <c r="B108">
+        <v>55</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108" t="b">
+        <v>0</v>
+      </c>
+      <c r="E108" t="b">
+        <v>0</v>
+      </c>
+      <c r="H108">
+        <v>0.872</v>
+      </c>
+      <c r="I108">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="J108">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="K108">
+        <v>0.85299999999999998</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" t="b">
+        <v>1</v>
+      </c>
+      <c r="B109">
+        <v>55</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="D109" t="b">
+        <v>0</v>
+      </c>
+      <c r="E109" t="b">
+        <v>0</v>
+      </c>
+      <c r="H109">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="I109">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="J109">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="K109">
+        <v>0.91300000000000003</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" t="b">
+        <v>1</v>
+      </c>
+      <c r="B110">
+        <v>55</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110" t="b">
+        <v>0</v>
+      </c>
+      <c r="E110" t="b">
+        <v>0</v>
+      </c>
+      <c r="H110">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="I110">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="J110">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="K110">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" t="b">
+        <v>1</v>
+      </c>
+      <c r="B111">
+        <v>55</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="D111" t="b">
+        <v>0</v>
+      </c>
+      <c r="E111" t="b">
+        <v>0</v>
+      </c>
+      <c r="H111">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="I111">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="J111">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="K111">
+        <v>0.86599999999999999</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" t="b">
+        <v>1</v>
+      </c>
+      <c r="B112">
+        <v>55</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="D112" t="b">
+        <v>0</v>
+      </c>
+      <c r="E112" t="b">
+        <v>0</v>
+      </c>
+      <c r="H112">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="I112">
+        <v>0.85</v>
+      </c>
+      <c r="J112">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="K112">
+        <v>0.89500000000000002</v>
+      </c>
+    </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
improved saving and loading results
</commit_message>
<xml_diff>
--- a/evaluation/training-evaluation.xlsx
+++ b/evaluation/training-evaluation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - University of Cyprus\ucl\thesis\workspace\cell-tracking-ucl-thesis\evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37092630-E0A8-4C48-9F81-390C4C89C9B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6F0351-2756-461A-9B57-9FC6673F4824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{DD5E1588-BB96-47E2-8F58-F1B1A8926599}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
   <si>
     <t>Standardise</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Mix Channel</t>
+  </si>
+  <si>
+    <t>drop confocal</t>
   </si>
 </sst>
 </file>
@@ -450,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25252485-713D-4CC8-BE64-95040359BD5A}">
-  <dimension ref="A1:Q150"/>
+  <dimension ref="A1:Q168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="H94" sqref="H94"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="G150" sqref="G150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -462,6 +465,7 @@
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.3671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.47265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.83984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.41796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.68359375" bestFit="1" customWidth="1"/>
@@ -3285,6 +3289,9 @@
       <c r="E131" t="s">
         <v>14</v>
       </c>
+      <c r="F131" t="s">
+        <v>16</v>
+      </c>
       <c r="H131" t="s">
         <v>4</v>
       </c>
@@ -3314,17 +3321,20 @@
       <c r="E132" t="b">
         <v>1</v>
       </c>
+      <c r="F132" t="b">
+        <v>0</v>
+      </c>
       <c r="H132">
-        <v>0.90300000000000002</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="I132">
         <v>0.84699999999999998</v>
       </c>
       <c r="J132">
-        <v>0.91800000000000004</v>
+        <v>0.88</v>
       </c>
       <c r="K132">
-        <v>0.86599999999999999</v>
+        <v>0.84199999999999997</v>
       </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3343,17 +3353,20 @@
       <c r="E133" t="b">
         <v>1</v>
       </c>
+      <c r="F133" t="b">
+        <v>0</v>
+      </c>
       <c r="H133">
-        <v>0.92500000000000004</v>
+        <v>0.89500000000000002</v>
       </c>
       <c r="I133">
         <v>0.85</v>
       </c>
       <c r="J133">
-        <v>0.92400000000000004</v>
+        <v>0.91400000000000003</v>
       </c>
       <c r="K133">
-        <v>0.89500000000000002</v>
+        <v>0.85799999999999998</v>
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3372,17 +3385,20 @@
       <c r="E134" t="b">
         <v>1</v>
       </c>
+      <c r="F134" t="b">
+        <v>0</v>
+      </c>
       <c r="H134">
-        <v>0.88600000000000001</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="I134">
-        <v>0.85199999999999998</v>
+        <v>0.84699999999999998</v>
       </c>
       <c r="J134">
-        <v>0.89200000000000002</v>
+        <v>0.89400000000000002</v>
       </c>
       <c r="K134">
-        <v>0.86699999999999999</v>
+        <v>0.89300000000000002</v>
       </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3401,17 +3417,20 @@
       <c r="E135" t="b">
         <v>1</v>
       </c>
+      <c r="F135" t="b">
+        <v>0</v>
+      </c>
       <c r="H135">
-        <v>0.88400000000000001</v>
+        <v>0.879</v>
       </c>
       <c r="I135">
-        <v>0.85</v>
+        <v>0.84499999999999997</v>
       </c>
       <c r="J135">
-        <v>0.9</v>
+        <v>0.91200000000000003</v>
       </c>
       <c r="K135">
-        <v>0.85399999999999998</v>
+        <v>0.83299999999999996</v>
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3430,17 +3449,20 @@
       <c r="E136" t="b">
         <v>1</v>
       </c>
+      <c r="F136" t="b">
+        <v>0</v>
+      </c>
       <c r="H136">
-        <v>0.9</v>
+        <v>0.90100000000000002</v>
       </c>
       <c r="I136">
-        <v>0.86</v>
+        <v>0.83299999999999996</v>
       </c>
       <c r="J136">
-        <v>0.91100000000000003</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="K136">
-        <v>0.873</v>
+        <v>0.91800000000000004</v>
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3459,17 +3481,20 @@
       <c r="E137" t="b">
         <v>1</v>
       </c>
+      <c r="F137" t="b">
+        <v>0</v>
+      </c>
       <c r="H137">
-        <v>0.88300000000000001</v>
+        <v>0.872</v>
       </c>
       <c r="I137">
-        <v>0.84399999999999997</v>
+        <v>0.84299999999999997</v>
       </c>
       <c r="J137">
-        <v>0.877</v>
+        <v>0.86199999999999999</v>
       </c>
       <c r="K137">
-        <v>0.873</v>
+        <v>0.871</v>
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3488,54 +3513,134 @@
       <c r="E138" t="b">
         <v>1</v>
       </c>
+      <c r="F138" t="b">
+        <v>0</v>
+      </c>
       <c r="H138">
-        <v>0.86099999999999999</v>
+        <v>0.89300000000000002</v>
       </c>
       <c r="I138">
-        <v>0.84399999999999997</v>
+        <v>0.85</v>
       </c>
       <c r="J138">
-        <v>0.82</v>
+        <v>0.89800000000000002</v>
       </c>
       <c r="K138">
-        <v>0.89600000000000002</v>
+        <v>0.871</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A139" t="b">
+        <v>1</v>
+      </c>
+      <c r="B139">
+        <v>31</v>
+      </c>
+      <c r="C139">
+        <v>0</v>
+      </c>
+      <c r="D139" t="b">
+        <v>0</v>
+      </c>
+      <c r="E139" t="b">
+        <v>1</v>
+      </c>
+      <c r="F139" t="b">
+        <v>0</v>
+      </c>
       <c r="H139">
-        <f>AVERAGE(H132:H138)</f>
-        <v>0.89171428571428568</v>
+        <v>0.872</v>
       </c>
       <c r="I139">
-        <f t="shared" ref="I139:K139" si="10">AVERAGE(I132:I138)</f>
-        <v>0.84957142857142876</v>
+        <v>0.85499999999999998</v>
       </c>
       <c r="J139">
-        <f t="shared" si="10"/>
-        <v>0.89171428571428568</v>
+        <v>0.86299999999999999</v>
       </c>
       <c r="K139">
-        <f t="shared" si="10"/>
-        <v>0.87485714285714289</v>
+        <v>0.874</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A140" t="b">
+        <v>1</v>
+      </c>
+      <c r="B140">
+        <v>31</v>
+      </c>
+      <c r="C140">
+        <v>0</v>
+      </c>
+      <c r="D140" t="b">
+        <v>0</v>
+      </c>
+      <c r="E140" t="b">
+        <v>1</v>
+      </c>
+      <c r="F140" t="b">
+        <v>0</v>
+      </c>
+      <c r="H140">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="I140">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="J140">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="K140">
+        <v>0.873</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141" t="b">
+        <v>1</v>
+      </c>
+      <c r="B141">
+        <v>31</v>
+      </c>
+      <c r="C141">
+        <v>0</v>
+      </c>
+      <c r="D141" t="b">
+        <v>0</v>
+      </c>
+      <c r="E141" t="b">
+        <v>1</v>
+      </c>
+      <c r="F141" t="b">
+        <v>0</v>
+      </c>
+      <c r="H141">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="I141">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="J141">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="K141">
+        <v>0.85199999999999998</v>
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A142" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A143" t="s">
-        <v>0</v>
-      </c>
-      <c r="B143" t="s">
-        <v>1</v>
-      </c>
-      <c r="C143" t="s">
-        <v>2</v>
-      </c>
-      <c r="D143" t="s">
-        <v>3</v>
+      <c r="H142">
+        <f>AVERAGE(H125:H131)</f>
+        <v>0.90566666666666673</v>
+      </c>
+      <c r="I142">
+        <f>AVERAGE(I125:I131)</f>
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="J142">
+        <f>AVERAGE(J125:J131)</f>
+        <v>0.90333333333333332</v>
+      </c>
+      <c r="K142">
+        <f>AVERAGE(K125:K131)</f>
+        <v>0.88700000000000001</v>
       </c>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -3543,96 +3648,471 @@
         <v>1</v>
       </c>
       <c r="B144">
+        <v>35</v>
+      </c>
+      <c r="C144">
+        <v>0</v>
+      </c>
+      <c r="D144" t="b">
+        <v>0</v>
+      </c>
+      <c r="E144" t="b">
+        <v>1</v>
+      </c>
+      <c r="F144" t="b">
+        <v>0</v>
+      </c>
+      <c r="H144">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="I144">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="J144">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="K144">
+        <v>0.89200000000000002</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A145" t="b">
+        <v>1</v>
+      </c>
+      <c r="B145">
+        <v>35</v>
+      </c>
+      <c r="C145">
+        <v>0</v>
+      </c>
+      <c r="D145" t="b">
+        <v>0</v>
+      </c>
+      <c r="E145" t="b">
+        <v>1</v>
+      </c>
+      <c r="F145" t="b">
+        <v>0</v>
+      </c>
+      <c r="H145">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="I145">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="J145">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="K145">
+        <v>0.879</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A146" t="b">
+        <v>1</v>
+      </c>
+      <c r="B146">
+        <v>35</v>
+      </c>
+      <c r="C146">
+        <v>0</v>
+      </c>
+      <c r="D146" t="b">
+        <v>0</v>
+      </c>
+      <c r="E146" t="b">
+        <v>1</v>
+      </c>
+      <c r="F146" t="b">
+        <v>0</v>
+      </c>
+      <c r="H146">
+        <v>0.88</v>
+      </c>
+      <c r="I146">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="J146">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="K146">
+        <v>0.86199999999999999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A147" t="b">
+        <v>1</v>
+      </c>
+      <c r="B147">
+        <v>35</v>
+      </c>
+      <c r="C147">
+        <v>0</v>
+      </c>
+      <c r="D147" t="b">
+        <v>0</v>
+      </c>
+      <c r="E147" t="b">
+        <v>1</v>
+      </c>
+      <c r="F147" t="b">
+        <v>0</v>
+      </c>
+      <c r="H147">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="I147">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="J147">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="K147">
+        <v>0.85299999999999998</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A148" t="b">
+        <v>1</v>
+      </c>
+      <c r="B148">
+        <v>35</v>
+      </c>
+      <c r="C148">
+        <v>0</v>
+      </c>
+      <c r="D148" t="b">
+        <v>0</v>
+      </c>
+      <c r="E148" t="b">
+        <v>1</v>
+      </c>
+      <c r="F148" t="b">
+        <v>0</v>
+      </c>
+      <c r="H148">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="I148">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="J148">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="K148">
+        <v>0.86099999999999999</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="H149">
+        <f>AVERAGE(H144:H148)</f>
+        <v>0.88000000000000012</v>
+      </c>
+      <c r="I149">
+        <f t="shared" ref="I149:K149" si="10">AVERAGE(I144:I148)</f>
+        <v>0.85419999999999996</v>
+      </c>
+      <c r="J149">
+        <f t="shared" si="10"/>
+        <v>0.88059999999999994</v>
+      </c>
+      <c r="K149">
+        <f t="shared" si="10"/>
+        <v>0.86939999999999995</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A151" t="b">
+        <v>1</v>
+      </c>
+      <c r="B151">
+        <v>27</v>
+      </c>
+      <c r="C151">
+        <v>0</v>
+      </c>
+      <c r="D151" t="b">
+        <v>0</v>
+      </c>
+      <c r="E151" t="b">
+        <v>1</v>
+      </c>
+      <c r="F151" t="b">
+        <v>0</v>
+      </c>
+      <c r="H151">
+        <v>0.876</v>
+      </c>
+      <c r="I151">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="J151">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="K151">
+        <v>0.88600000000000001</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A152" t="b">
+        <v>1</v>
+      </c>
+      <c r="B152">
+        <v>27</v>
+      </c>
+      <c r="C152">
+        <v>0</v>
+      </c>
+      <c r="D152" t="b">
+        <v>0</v>
+      </c>
+      <c r="E152" t="b">
+        <v>1</v>
+      </c>
+      <c r="F152" t="b">
+        <v>0</v>
+      </c>
+      <c r="H152">
+        <v>0.88</v>
+      </c>
+      <c r="I152">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="J152">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="K152">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A153" t="b">
+        <v>1</v>
+      </c>
+      <c r="B153">
+        <v>27</v>
+      </c>
+      <c r="C153">
+        <v>0</v>
+      </c>
+      <c r="D153" t="b">
+        <v>0</v>
+      </c>
+      <c r="E153" t="b">
+        <v>1</v>
+      </c>
+      <c r="F153" t="b">
+        <v>0</v>
+      </c>
+      <c r="H153">
+        <v>0.874</v>
+      </c>
+      <c r="I153">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="J153">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="K153">
+        <v>0.877</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A154" t="b">
+        <v>1</v>
+      </c>
+      <c r="B154">
+        <v>27</v>
+      </c>
+      <c r="C154">
+        <v>0</v>
+      </c>
+      <c r="D154" t="b">
+        <v>0</v>
+      </c>
+      <c r="E154" t="b">
+        <v>1</v>
+      </c>
+      <c r="F154" t="b">
+        <v>0</v>
+      </c>
+      <c r="H154">
+        <v>0.873</v>
+      </c>
+      <c r="I154">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="J154">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="K154">
+        <v>0.89900000000000002</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A155" t="b">
+        <v>1</v>
+      </c>
+      <c r="B155">
+        <v>27</v>
+      </c>
+      <c r="C155">
+        <v>0</v>
+      </c>
+      <c r="D155" t="b">
+        <v>0</v>
+      </c>
+      <c r="E155" t="b">
+        <v>1</v>
+      </c>
+      <c r="F155" t="b">
+        <v>0</v>
+      </c>
+      <c r="H155">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="I155">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="J155">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="K155">
+        <v>0.85399999999999998</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="H156">
+        <f>AVERAGE(H151:H155)</f>
+        <v>0.87740000000000007</v>
+      </c>
+      <c r="I156">
+        <f t="shared" ref="I156:K156" si="11">AVERAGE(I151:I155)</f>
+        <v>0.84439999999999993</v>
+      </c>
+      <c r="J156">
+        <f t="shared" si="11"/>
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="K156">
+        <f t="shared" si="11"/>
+        <v>0.87319999999999998</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A160" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A161" t="s">
+        <v>0</v>
+      </c>
+      <c r="B161" t="s">
+        <v>1</v>
+      </c>
+      <c r="C161" t="s">
+        <v>2</v>
+      </c>
+      <c r="D161" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A162" t="b">
+        <v>1</v>
+      </c>
+      <c r="B162">
         <v>21</v>
       </c>
-      <c r="C144">
-        <v>0</v>
-      </c>
-      <c r="D144" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A145" t="b">
-        <v>1</v>
-      </c>
-      <c r="B145">
+      <c r="C162">
+        <v>0</v>
+      </c>
+      <c r="D162" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A163" t="b">
+        <v>1</v>
+      </c>
+      <c r="B163">
         <v>21</v>
       </c>
-      <c r="C145">
-        <v>0</v>
-      </c>
-      <c r="D145" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A146" t="b">
-        <v>1</v>
-      </c>
-      <c r="B146">
+      <c r="C163">
+        <v>0</v>
+      </c>
+      <c r="D163" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A164" t="b">
+        <v>1</v>
+      </c>
+      <c r="B164">
         <v>21</v>
       </c>
-      <c r="C146">
-        <v>0</v>
-      </c>
-      <c r="D146" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A147" t="b">
-        <v>1</v>
-      </c>
-      <c r="B147">
+      <c r="C164">
+        <v>0</v>
+      </c>
+      <c r="D164" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A165" t="b">
+        <v>1</v>
+      </c>
+      <c r="B165">
         <v>21</v>
       </c>
-      <c r="C147">
-        <v>0</v>
-      </c>
-      <c r="D147" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A148" t="b">
-        <v>1</v>
-      </c>
-      <c r="B148">
+      <c r="C165">
+        <v>0</v>
+      </c>
+      <c r="D165" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A166" t="b">
+        <v>1</v>
+      </c>
+      <c r="B166">
         <v>21</v>
       </c>
-      <c r="C148">
-        <v>0</v>
-      </c>
-      <c r="D148" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A149" t="b">
-        <v>1</v>
-      </c>
-      <c r="B149">
+      <c r="C166">
+        <v>0</v>
+      </c>
+      <c r="D166" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A167" t="b">
+        <v>1</v>
+      </c>
+      <c r="B167">
         <v>21</v>
       </c>
-      <c r="C149">
-        <v>0</v>
-      </c>
-      <c r="D149" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A150" t="b">
-        <v>1</v>
-      </c>
-      <c r="B150">
+      <c r="C167">
+        <v>0</v>
+      </c>
+      <c r="D167" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A168" t="b">
+        <v>1</v>
+      </c>
+      <c r="B168">
         <v>21</v>
       </c>
-      <c r="C150">
-        <v>0</v>
-      </c>
-      <c r="D150" t="b">
+      <c r="C168">
+        <v>0</v>
+      </c>
+      <c r="D168" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>